<commit_message>
fixed iloc[:, 2] to be iloc[i:, 2]; and used pd.isna to check 'None'
</commit_message>
<xml_diff>
--- a/pdtest1.xlsx
+++ b/pdtest1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phe\Documents\tech\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB00D0B-BB0A-4B7A-A740-C9300EFEDB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F756970-E068-4824-9294-2A0E1575C61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="14610" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="20850" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>